<commit_message>
Dockerized OCHRE (with conda). Integrated with Gridlab-D for so-simulation.
</commit_message>
<xml_diff>
--- a/inputs/MS/Main_spreadsheet_test40_original.xlsx
+++ b/inputs/MS/Main_spreadsheet_test40_original.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pmunanka/Documents/projects/fastderms/repos/Co-Simulation/inputs/MS/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wang314\Code_Data\fastderms_cosim\inputs\MS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06A99A47-7BF3-8B46-9C31-30715CAF3864}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86FBF705-0FE7-402A-9646-C54F189B741D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6200" yWindow="2900" windowWidth="35840" windowHeight="18380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2660" yWindow="2660" windowWidth="28800" windowHeight="15460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DOOM Input file data" sheetId="2" r:id="rId1"/>
@@ -152,96 +152,6 @@
     <t>n30</t>
   </si>
   <si>
-    <t>load_1_p2ulv10359</t>
-  </si>
-  <si>
-    <t>load_1_p2ulv34367</t>
-  </si>
-  <si>
-    <t>load_1_p2ulv10358</t>
-  </si>
-  <si>
-    <t>load_1_p2ulv10350</t>
-  </si>
-  <si>
-    <t>load_1_p2ulv10349</t>
-  </si>
-  <si>
-    <t>load_1_p2ulv10372</t>
-  </si>
-  <si>
-    <t>load_1_p2ulv10371</t>
-  </si>
-  <si>
-    <t>load_1_p2ulv10370</t>
-  </si>
-  <si>
-    <t>load_1_p2ulv10369</t>
-  </si>
-  <si>
-    <t>load_1_p2ulv4847</t>
-  </si>
-  <si>
-    <t>load_2_p2ulv10359</t>
-  </si>
-  <si>
-    <t>load_2_p2ulv34367</t>
-  </si>
-  <si>
-    <t>load_2_p2ulv10358</t>
-  </si>
-  <si>
-    <t>load_2_p2ulv10350</t>
-  </si>
-  <si>
-    <t>load_2_p2ulv10349</t>
-  </si>
-  <si>
-    <t>load_2_p2ulv10372</t>
-  </si>
-  <si>
-    <t>load_2_p2ulv10371</t>
-  </si>
-  <si>
-    <t>load_2_p2ulv10370</t>
-  </si>
-  <si>
-    <t>load_2_p2ulv10369</t>
-  </si>
-  <si>
-    <t>load_2_p2ulv4847</t>
-  </si>
-  <si>
-    <t>load_3_p2ulv10359</t>
-  </si>
-  <si>
-    <t>load_3_p2ulv34367</t>
-  </si>
-  <si>
-    <t>load_3_p2ulv10358</t>
-  </si>
-  <si>
-    <t>load_3_p2ulv10350</t>
-  </si>
-  <si>
-    <t>load_3_p2ulv10349</t>
-  </si>
-  <si>
-    <t>load_3_p2ulv10372</t>
-  </si>
-  <si>
-    <t>load_3_p2ulv10371</t>
-  </si>
-  <si>
-    <t>load_3_p2ulv10370</t>
-  </si>
-  <si>
-    <t>load_3_p2ulv10369</t>
-  </si>
-  <si>
-    <t>load_3_p2ulv4847</t>
-  </si>
-  <si>
     <t>n31</t>
   </si>
   <si>
@@ -272,34 +182,124 @@
     <t>n40</t>
   </si>
   <si>
-    <t>load_4_p2ulv10359</t>
-  </si>
-  <si>
-    <t>load_4_p2ulv34367</t>
-  </si>
-  <si>
-    <t>load_4_p2ulv10358</t>
-  </si>
-  <si>
-    <t>load_4_p2ulv10350</t>
-  </si>
-  <si>
-    <t>load_4_p2ulv10349</t>
-  </si>
-  <si>
-    <t>load_4_p2ulv10372</t>
-  </si>
-  <si>
-    <t>load_4_p2ulv10371</t>
-  </si>
-  <si>
-    <t>load_4_p2ulv10370</t>
-  </si>
-  <si>
-    <t>load_4_p2ulv10369</t>
-  </si>
-  <si>
-    <t>load_4_p2ulv4847</t>
+    <t>tl_house_1</t>
+  </si>
+  <si>
+    <t>tl_house_2</t>
+  </si>
+  <si>
+    <t>tl_house_3</t>
+  </si>
+  <si>
+    <t>tl_house_4</t>
+  </si>
+  <si>
+    <t>tl_house_5</t>
+  </si>
+  <si>
+    <t>tl_house_6</t>
+  </si>
+  <si>
+    <t>tl_house_7</t>
+  </si>
+  <si>
+    <t>tl_house_8</t>
+  </si>
+  <si>
+    <t>tl_house_9</t>
+  </si>
+  <si>
+    <t>tl_house_10</t>
+  </si>
+  <si>
+    <t>tl_house_11</t>
+  </si>
+  <si>
+    <t>tl_house_12</t>
+  </si>
+  <si>
+    <t>tl_house_13</t>
+  </si>
+  <si>
+    <t>tl_house_14</t>
+  </si>
+  <si>
+    <t>tl_house_15</t>
+  </si>
+  <si>
+    <t>tl_house_16</t>
+  </si>
+  <si>
+    <t>tl_house_17</t>
+  </si>
+  <si>
+    <t>tl_house_18</t>
+  </si>
+  <si>
+    <t>tl_house_19</t>
+  </si>
+  <si>
+    <t>tl_house_20</t>
+  </si>
+  <si>
+    <t>tl_house_21</t>
+  </si>
+  <si>
+    <t>tl_house_22</t>
+  </si>
+  <si>
+    <t>tl_house_23</t>
+  </si>
+  <si>
+    <t>tl_house_24</t>
+  </si>
+  <si>
+    <t>tl_house_25</t>
+  </si>
+  <si>
+    <t>tl_house_26</t>
+  </si>
+  <si>
+    <t>tl_house_27</t>
+  </si>
+  <si>
+    <t>tl_house_28</t>
+  </si>
+  <si>
+    <t>tl_house_29</t>
+  </si>
+  <si>
+    <t>tl_house_30</t>
+  </si>
+  <si>
+    <t>tl_house_31</t>
+  </si>
+  <si>
+    <t>tl_house_32</t>
+  </si>
+  <si>
+    <t>tl_house_33</t>
+  </si>
+  <si>
+    <t>tl_house_34</t>
+  </si>
+  <si>
+    <t>tl_house_35</t>
+  </si>
+  <si>
+    <t>tl_house_36</t>
+  </si>
+  <si>
+    <t>tl_house_37</t>
+  </si>
+  <si>
+    <t>tl_house_38</t>
+  </si>
+  <si>
+    <t>tl_house_39</t>
+  </si>
+  <si>
+    <t>tl_house_40</t>
   </si>
 </sst>
 </file>
@@ -1172,19 +1172,19 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E6" sqref="E6"/>
+      <selection pane="bottomRight" activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="5.33203125" customWidth="1"/>
-    <col min="3" max="3" width="20.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.5" customWidth="1"/>
-    <col min="6" max="6" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="5.36328125" customWidth="1"/>
+    <col min="3" max="3" width="20.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.453125" customWidth="1"/>
+    <col min="6" max="6" width="25.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -1204,7 +1204,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -1222,10 +1222,10 @@
         <v>3</v>
       </c>
       <c r="F2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -1243,10 +1243,10 @@
         <v>5</v>
       </c>
       <c r="F3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -1264,10 +1264,10 @@
         <v>4</v>
       </c>
       <c r="F4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -1285,10 +1285,10 @@
         <v>3</v>
       </c>
       <c r="F5" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -1306,10 +1306,10 @@
         <v>3</v>
       </c>
       <c r="F6" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -1327,10 +1327,10 @@
         <v>4</v>
       </c>
       <c r="F7" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -1348,10 +1348,10 @@
         <v>3</v>
       </c>
       <c r="F8" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -1369,10 +1369,10 @@
         <v>4</v>
       </c>
       <c r="F9" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -1390,10 +1390,10 @@
         <v>2</v>
       </c>
       <c r="F10" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -1411,10 +1411,10 @@
         <v>3</v>
       </c>
       <c r="F11" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -1432,10 +1432,10 @@
         <v>3</v>
       </c>
       <c r="F12" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -1453,10 +1453,10 @@
         <v>2</v>
       </c>
       <c r="F13" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -1474,10 +1474,10 @@
         <v>3</v>
       </c>
       <c r="F14" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -1495,10 +1495,10 @@
         <v>3</v>
       </c>
       <c r="F15" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -1516,10 +1516,10 @@
         <v>3</v>
       </c>
       <c r="F16" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -1537,10 +1537,10 @@
         <v>3</v>
       </c>
       <c r="F17" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -1558,10 +1558,10 @@
         <v>4</v>
       </c>
       <c r="F18" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -1579,10 +1579,10 @@
         <v>2</v>
       </c>
       <c r="F19" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -1600,10 +1600,10 @@
         <v>3</v>
       </c>
       <c r="F20" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" s="3">
         <v>20</v>
       </c>
@@ -1621,10 +1621,10 @@
         <v>2</v>
       </c>
       <c r="F21" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" s="3">
         <v>21</v>
       </c>
@@ -1642,10 +1642,10 @@
         <v>4</v>
       </c>
       <c r="F22" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" s="2">
         <v>22</v>
       </c>
@@ -1663,10 +1663,10 @@
         <v>3</v>
       </c>
       <c r="F23" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" s="2">
         <v>23</v>
       </c>
@@ -1684,10 +1684,10 @@
         <v>2</v>
       </c>
       <c r="F24" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" s="3">
         <v>24</v>
       </c>
@@ -1705,10 +1705,10 @@
         <v>3</v>
       </c>
       <c r="F25" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" s="3">
         <v>25</v>
       </c>
@@ -1726,10 +1726,10 @@
         <v>3</v>
       </c>
       <c r="F26" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" s="3">
         <v>26</v>
       </c>
@@ -1747,10 +1747,10 @@
         <v>5</v>
       </c>
       <c r="F27" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" s="3">
         <v>27</v>
       </c>
@@ -1768,10 +1768,10 @@
         <v>3</v>
       </c>
       <c r="F28" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" s="2">
         <v>28</v>
       </c>
@@ -1789,10 +1789,10 @@
         <v>3</v>
       </c>
       <c r="F29" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" s="3">
         <v>29</v>
       </c>
@@ -1810,10 +1810,10 @@
         <v>3</v>
       </c>
       <c r="F30" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31" s="3">
         <v>30</v>
       </c>
@@ -1831,15 +1831,15 @@
         <v>3</v>
       </c>
       <c r="F31" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32" s="3">
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>70</v>
+        <v>40</v>
       </c>
       <c r="C32" t="str">
         <f t="shared" si="0"/>
@@ -1855,12 +1855,12 @@
         <v>80</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33" s="3">
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>71</v>
+        <v>41</v>
       </c>
       <c r="C33" t="str">
         <f t="shared" si="0"/>
@@ -1876,12 +1876,12 @@
         <v>81</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A34" s="3">
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>72</v>
+        <v>42</v>
       </c>
       <c r="C34" t="str">
         <f t="shared" si="0"/>
@@ -1897,12 +1897,12 @@
         <v>82</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A35" s="3">
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>73</v>
+        <v>43</v>
       </c>
       <c r="C35" t="str">
         <f t="shared" si="0"/>
@@ -1918,12 +1918,12 @@
         <v>83</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A36" s="3">
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>74</v>
+        <v>44</v>
       </c>
       <c r="C36" t="str">
         <f t="shared" si="0"/>
@@ -1939,12 +1939,12 @@
         <v>84</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37" s="3">
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>75</v>
+        <v>45</v>
       </c>
       <c r="C37" t="str">
         <f t="shared" si="0"/>
@@ -1960,12 +1960,12 @@
         <v>85</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A38" s="3">
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>76</v>
+        <v>46</v>
       </c>
       <c r="C38" t="str">
         <f t="shared" si="0"/>
@@ -1981,12 +1981,12 @@
         <v>86</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A39" s="3">
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>77</v>
+        <v>47</v>
       </c>
       <c r="C39" t="str">
         <f t="shared" si="0"/>
@@ -2002,12 +2002,12 @@
         <v>87</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A40" s="3">
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>78</v>
+        <v>48</v>
       </c>
       <c r="C40" t="str">
         <f t="shared" si="0"/>
@@ -2023,12 +2023,12 @@
         <v>88</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A41" s="3">
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>79</v>
+        <v>49</v>
       </c>
       <c r="C41" t="str">
         <f t="shared" si="0"/>

</xml_diff>